<commit_message>
Change number of fees
</commit_message>
<xml_diff>
--- a/public/imports/promesas.xlsx
+++ b/public/imports/promesas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rivarca\public\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36906C1C-0DBC-4370-81AD-32B08DD0B930}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425440B1-F259-4D52-B47A-30607A3187F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{DD919BFB-7F5D-47AC-9A0A-D4F6AAD42B29}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2917" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2914" uniqueCount="863">
   <si>
     <t xml:space="preserve">MANZANA </t>
   </si>
@@ -2967,8 +2967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EB9583-E0A2-4347-8D1B-17D688AB9D0D}">
   <dimension ref="A1:AB346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G331" workbookViewId="0">
-      <selection activeCell="V220" sqref="V220"/>
+    <sheetView tabSelected="1" topLeftCell="N332" workbookViewId="0">
+      <selection activeCell="AA323" sqref="AA323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2976,6 +2976,10 @@
     <col min="15" max="15" width="18.140625" customWidth="1"/>
     <col min="22" max="22" width="40.28515625" customWidth="1"/>
     <col min="23" max="23" width="28.42578125" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" customWidth="1"/>
+    <col min="26" max="26" width="22" customWidth="1"/>
+    <col min="27" max="27" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -6568,9 +6572,6 @@
       <c r="Z102" t="s">
         <v>165</v>
       </c>
-      <c r="AA102" t="s">
-        <v>166</v>
-      </c>
       <c r="AB102" t="s">
         <v>167</v>
       </c>
@@ -16629,9 +16630,6 @@
       <c r="Z322" t="s">
         <v>260</v>
       </c>
-      <c r="AA322" t="s">
-        <v>166</v>
-      </c>
       <c r="AB322" t="s">
         <v>772</v>
       </c>
@@ -16699,9 +16697,6 @@
       </c>
       <c r="Z323" t="s">
         <v>260</v>
-      </c>
-      <c r="AA323" t="s">
-        <v>166</v>
       </c>
       <c r="AB323" t="s">
         <v>772</v>

</xml_diff>